<commit_message>
map dto to entity
</commit_message>
<xml_diff>
--- a/doc/技术问题记录.xlsx
+++ b/doc/技术问题记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5610" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5610"/>
   </bookViews>
   <sheets>
     <sheet name="技术问题记录" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>问题</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -258,6 +258,14 @@
   </si>
   <si>
     <t>情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用MapStruct映射DTO与数据库实体Entity之间，总不容易映射符合要求。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mapper中要用上uses,Entity中要加上关联表的实体，DTO中则只是声明关联表的一个小的数据对象，也是一个DTO.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -338,14 +346,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -620,7 +628,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -695,6 +703,14 @@
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="40.5">
+      <c r="A6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -731,10 +747,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
@@ -742,36 +758,36 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
@@ -779,23 +795,23 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4"/>
+      <c r="A9" s="6"/>
       <c r="B9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C10" t="s">
@@ -803,29 +819,29 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
       <c r="C11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
       <c r="C12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
       <c r="C13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C14" t="s">
@@ -833,12 +849,12 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C16" t="s">
@@ -846,21 +862,21 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
       <c r="C17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
       <c r="C18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B19" t="s">
@@ -868,13 +884,13 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="6"/>
       <c r="B20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="6"/>
       <c r="B21" t="s">
         <v>36</v>
       </c>
@@ -933,7 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -975,10 +991,10 @@
       <c r="A1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>